<commit_message>
Xây dựng giao diện Footer Bottom
</commit_message>
<xml_diff>
--- a/me/3.project/7.Xay-dung-giao-dien-Footer.xlsx
+++ b/me/3.project/7.Xay-dung-giao-dien-Footer.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\sass-gruntjs-bootstrap\me\3.project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E88A9835-BDBD-434B-8EA6-74D26085C977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89A94E83-ACF5-4EDE-852E-E0C77F4E9ACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Footer Top" sheetId="1" r:id="rId1"/>
+    <sheet name="Footer Bottom" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="428">
   <si>
     <t>構成</t>
   </si>
@@ -1186,6 +1187,129 @@
   </si>
   <si>
     <t>    @include setFooterTop(12px);</t>
+  </si>
+  <si>
+    <t>_footer-bottom.scss</t>
+  </si>
+  <si>
+    <t>    &lt;!-- FOOTER BOTTOM : START --&gt;</t>
+  </si>
+  <si>
+    <t>    &lt;div class="footer-bottom"&gt;</t>
+  </si>
+  <si>
+    <t>            &lt;!-- CopyRight --&gt;</t>
+  </si>
+  <si>
+    <t>            &lt;div class="copyright pull-left"&gt;</t>
+  </si>
+  <si>
+    <t>                &lt;p&gt;&amp;#169; All rights reserved | Template by&amp;nbsp;&lt;a href="#"&gt; W3Layouts&lt;/a&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>            &lt;!-- Social Icons --&gt;</t>
+  </si>
+  <si>
+    <t>            &lt;div class="social-icons pull-right "&gt;</t>
+  </si>
+  <si>
+    <t>                &lt;ul class="list-unstyled"&gt;</t>
+  </si>
+  <si>
+    <t>                    &lt;li&gt;&lt;a href="#"&gt;&lt;i class="fa fa-twitter"&gt;&lt;/i&gt;&lt;/a&gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>                    &lt;li&gt;&lt;a href="#"&gt;&lt;i class="fa fa-facebook"&gt;&lt;/i&gt;&lt;/a&gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>                    &lt;li&gt;&lt;a href="#"&gt;&lt;i class="fa fa-google-plus"&gt;&lt;/i&gt;&lt;/a&gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>                    &lt;li&gt;&lt;a href="#"&gt;&lt;i class="fa fa-rss"&gt;&lt;/i&gt;&lt;/a&gt;&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>                &lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>    &lt;!-- FOOTER BOTTOM : END --&gt;</t>
+  </si>
+  <si>
+    <t>development\sass\footer\_footer-bottom.scss</t>
+  </si>
+  <si>
+    <t>div.footer-bottom {</t>
+  </si>
+  <si>
+    <t>    background-color: #6AB3AC;</t>
+  </si>
+  <si>
+    <t>    padding: 2% 0;</t>
+  </si>
+  <si>
+    <t>    div.social-icons {</t>
+  </si>
+  <si>
+    <t>        ul {</t>
+  </si>
+  <si>
+    <t>            li {</t>
+  </si>
+  <si>
+    <t>                text-align: center;</t>
+  </si>
+  <si>
+    <t>                margin-left: 20px;</t>
+  </si>
+  <si>
+    <t>                    display: inline-block;</t>
+  </si>
+  <si>
+    <t>                    i {</t>
+  </si>
+  <si>
+    <t>                        @include setFont(24px, $color-white);</t>
+  </si>
+  <si>
+    <t>                    &amp;:hover i{</t>
+  </si>
+  <si>
+    <t>                        color: #E8645A;</t>
+  </si>
+  <si>
+    <t>    div.copyright {</t>
+  </si>
+  <si>
+    <t>        p {</t>
+  </si>
+  <si>
+    <t>            @include setFont(14px, $color-white);</t>
+  </si>
+  <si>
+    <t>            @include setTagAHover(#E2534B, $color-white);</t>
+  </si>
+  <si>
+    <t>    @import "footer-bottom";</t>
+  </si>
+  <si>
+    <t>_mixin.scss này chứa định dạng cho nó hiển thị tốt trên các loại thiết bị</t>
+  </si>
+  <si>
+    <t>Chứa các mixin sử dụng đi sử dụng lại đối với toàn bộ folder sass</t>
+  </si>
+  <si>
+    <t>// Footer Bottom</t>
+  </si>
+  <si>
+    <t>@mixin setFooterBottom() {</t>
+  </si>
+  <si>
+    <t>    div.footer-bottom {</t>
+  </si>
+  <si>
+    <t>        div.copyright, div.social-icons {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    @include setFooterBottom(); </t>
   </si>
 </sst>
 </file>
@@ -3105,6 +3229,381 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>124</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>162</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A84AED87-CD1D-EF47-E496-FE84A4484269}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1428750" y="23774400"/>
+          <a:ext cx="523875" cy="7143750"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>85726</xdr:colOff>
+      <xdr:row>126</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>343178</xdr:colOff>
+      <xdr:row>156</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B2DE91B-D10F-4FBC-A214-DC8C0B933A3E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8010526" y="24107775"/>
+          <a:ext cx="11230252" cy="5753100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>154</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{741532A3-1856-49E0-8625-1E3DD3304377}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4886325" y="29146500"/>
+          <a:ext cx="3686175" cy="285750"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>139</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27A9C5D2-3AFD-5E8E-9C2C-054ECDF4D066}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4886325" y="26489025"/>
+          <a:ext cx="11820525" cy="2819400"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>288</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>307</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF858CD1-DDB5-36A4-0BE2-6138DBC8AEC2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="1733550" y="55025925"/>
+          <a:ext cx="171450" cy="3524250"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>278</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>456388</xdr:colOff>
+      <xdr:row>295</xdr:row>
+      <xdr:rowOff>171037</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9EB3E943-2648-65D7-877E-4AA8F9E66432}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7372350" y="53063775"/>
+          <a:ext cx="6495238" cy="3304762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>288</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>291</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Straight Arrow Connector 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{480B857C-D13D-576C-F2AD-16F36A2D440D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="6115050" y="55006875"/>
+          <a:ext cx="3695700" cy="428625"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3370,8 +3869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:AE585"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A560" workbookViewId="0">
-      <selection activeCell="J579" sqref="J579"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:I73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10159,4 +10658,3763 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F410826-5F9D-4555-9EE8-2FEEC4D3F519}">
+  <dimension ref="A2:M309"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A301" workbookViewId="0">
+      <selection activeCell="M314" sqref="M314"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="10"/>
+      <c r="B3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="13"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="15"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="15"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="10"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="15"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="10"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="15"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="10"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="15"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="10"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="15"/>
+      <c r="J9" t="s">
+        <v>55</v>
+      </c>
+      <c r="K9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="10"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="15"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="10"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="15"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="10"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="15"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="10"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="15"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="10"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="15"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="10"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="15"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="10"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="15"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="10"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="15"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="10"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="15"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="10"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="15"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="10"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="15"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="10"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H21" s="10"/>
+      <c r="I21" s="15"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="10"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="10"/>
+      <c r="I22" s="15"/>
+      <c r="J22" t="s">
+        <v>55</v>
+      </c>
+      <c r="K22" t="s">
+        <v>63</v>
+      </c>
+      <c r="M22" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="10"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23" s="10"/>
+      <c r="I23" s="15"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="10"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H24" s="10"/>
+      <c r="I24" s="15"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="10"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H25" s="10"/>
+      <c r="I25" s="15"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="10"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H26" s="10"/>
+      <c r="I26" s="15"/>
+      <c r="J26" t="s">
+        <v>55</v>
+      </c>
+      <c r="K26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="10"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H27" s="10"/>
+      <c r="I27" s="15"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="10"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="15"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="10"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="H29" s="10"/>
+      <c r="I29" s="15"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="10"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H30" s="10"/>
+      <c r="I30" s="15"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="10"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H31" s="10"/>
+      <c r="I31" s="15"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="10"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="15"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="10"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="6" t="s">
+        <v>387</v>
+      </c>
+      <c r="H33" s="10"/>
+      <c r="I33" s="15"/>
+      <c r="J33" t="s">
+        <v>55</v>
+      </c>
+      <c r="K33" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" s="10"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="H34" s="10"/>
+      <c r="I34" s="15"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" s="10"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H35" s="10"/>
+      <c r="I35" s="15"/>
+      <c r="J35" t="s">
+        <v>55</v>
+      </c>
+      <c r="K35" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" s="10"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="15"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" s="10"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H37" s="10"/>
+      <c r="I37" s="15"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" s="10"/>
+      <c r="B38" s="14"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="H38" s="10"/>
+      <c r="I38" s="15"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" s="10"/>
+      <c r="B39" s="14"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H39" s="10"/>
+      <c r="I39" s="15"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" s="10"/>
+      <c r="B40" s="14"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="15"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" s="10"/>
+      <c r="B41" s="14"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H41" s="10"/>
+      <c r="I41" s="15"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" s="10"/>
+      <c r="B42" s="14"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="H42" s="10"/>
+      <c r="I42" s="15"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43" s="10"/>
+      <c r="B43" s="14"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H43" s="10"/>
+      <c r="I43" s="15"/>
+      <c r="M43" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44" s="10"/>
+      <c r="B44" s="14"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="G44" s="10"/>
+      <c r="H44" s="10"/>
+      <c r="I44" s="15"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45" s="10"/>
+      <c r="B45" s="14"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H45" s="10"/>
+      <c r="I45" s="15"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" s="10"/>
+      <c r="B46" s="14"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="10"/>
+      <c r="G46" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="H46" s="10"/>
+      <c r="I46" s="15"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" s="10"/>
+      <c r="B47" s="14"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="10"/>
+      <c r="F47" s="10"/>
+      <c r="G47" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H47" s="10"/>
+      <c r="I47" s="15"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" s="10"/>
+      <c r="B48" s="14"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="10"/>
+      <c r="F48" s="10"/>
+      <c r="G48" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H48" s="10"/>
+      <c r="I48" s="15"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="10"/>
+      <c r="B49" s="14"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="10"/>
+      <c r="G49" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="H49" s="10"/>
+      <c r="I49" s="15"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="10"/>
+      <c r="B50" s="14"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="10"/>
+      <c r="F50" s="10"/>
+      <c r="G50" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H50" s="10"/>
+      <c r="I50" s="15"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="10"/>
+      <c r="B51" s="14"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="10"/>
+      <c r="E51" s="10"/>
+      <c r="F51" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G51" s="10"/>
+      <c r="H51" s="10"/>
+      <c r="I51" s="15"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="10"/>
+      <c r="B52" s="14"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="10"/>
+      <c r="E52" s="10"/>
+      <c r="F52" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="G52" s="10"/>
+      <c r="H52" s="10"/>
+      <c r="I52" s="15"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="10"/>
+      <c r="B53" s="14"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="10"/>
+      <c r="E53" s="10"/>
+      <c r="F53" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G53" s="10"/>
+      <c r="H53" s="10"/>
+      <c r="I53" s="15"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="10"/>
+      <c r="B54" s="14"/>
+      <c r="C54" s="10"/>
+      <c r="D54" s="10"/>
+      <c r="E54" s="10"/>
+      <c r="F54" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G54" s="10"/>
+      <c r="H54" s="10"/>
+      <c r="I54" s="15"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="10"/>
+      <c r="B55" s="14"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="10"/>
+      <c r="E55" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F55" s="10"/>
+      <c r="G55" s="10"/>
+      <c r="H55" s="10"/>
+      <c r="I55" s="15"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="10"/>
+      <c r="B56" s="14"/>
+      <c r="C56" s="10"/>
+      <c r="D56" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E56" s="10"/>
+      <c r="F56" s="10"/>
+      <c r="G56" s="10"/>
+      <c r="H56" s="10"/>
+      <c r="I56" s="15"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="10"/>
+      <c r="B57" s="14"/>
+      <c r="C57" s="10"/>
+      <c r="D57" s="10"/>
+      <c r="E57" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F57" s="10"/>
+      <c r="G57" s="10"/>
+      <c r="H57" s="10"/>
+      <c r="I57" s="15"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="10"/>
+      <c r="B58" s="14"/>
+      <c r="C58" s="10"/>
+      <c r="D58" s="10"/>
+      <c r="E58" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F58" s="10"/>
+      <c r="G58" s="10"/>
+      <c r="H58" s="10"/>
+      <c r="I58" s="15"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="10"/>
+      <c r="B59" s="14"/>
+      <c r="C59" s="10"/>
+      <c r="D59" s="10"/>
+      <c r="E59" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F59" s="10"/>
+      <c r="G59" s="10"/>
+      <c r="H59" s="10"/>
+      <c r="I59" s="15"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="10"/>
+      <c r="B60" s="14"/>
+      <c r="C60" s="10"/>
+      <c r="D60" s="10"/>
+      <c r="E60" s="10"/>
+      <c r="F60" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="G60" s="10"/>
+      <c r="H60" s="10"/>
+      <c r="I60" s="15"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="10"/>
+      <c r="B61" s="14"/>
+      <c r="C61" s="10"/>
+      <c r="D61" s="10"/>
+      <c r="E61" s="10"/>
+      <c r="F61" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G61" s="10"/>
+      <c r="H61" s="10"/>
+      <c r="I61" s="15"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="10"/>
+      <c r="B62" s="14"/>
+      <c r="C62" s="10"/>
+      <c r="D62" s="10"/>
+      <c r="E62" s="10"/>
+      <c r="F62" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G62" s="10"/>
+      <c r="H62" s="10"/>
+      <c r="I62" s="15"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="10"/>
+      <c r="B63" s="14"/>
+      <c r="C63" s="10"/>
+      <c r="D63" s="10"/>
+      <c r="E63" s="10"/>
+      <c r="F63" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="G63" s="10"/>
+      <c r="H63" s="10"/>
+      <c r="I63" s="15"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="10"/>
+      <c r="B64" s="14"/>
+      <c r="C64" s="10"/>
+      <c r="D64" s="10"/>
+      <c r="E64" s="10"/>
+      <c r="F64" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G64" s="10"/>
+      <c r="H64" s="10"/>
+      <c r="I64" s="15"/>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A65" s="10"/>
+      <c r="B65" s="14"/>
+      <c r="C65" s="10"/>
+      <c r="D65" s="10"/>
+      <c r="E65" s="10"/>
+      <c r="F65" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G65" s="10"/>
+      <c r="H65" s="10"/>
+      <c r="I65" s="15"/>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A66" s="10"/>
+      <c r="B66" s="14"/>
+      <c r="C66" s="10"/>
+      <c r="D66" s="10"/>
+      <c r="E66" s="10"/>
+      <c r="F66" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G66" s="10"/>
+      <c r="H66" s="10"/>
+      <c r="I66" s="15"/>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A67" s="10"/>
+      <c r="B67" s="14"/>
+      <c r="C67" s="10"/>
+      <c r="D67" s="10"/>
+      <c r="E67" s="10"/>
+      <c r="F67" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="G67" s="10"/>
+      <c r="H67" s="10"/>
+      <c r="I67" s="15"/>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A68" s="10"/>
+      <c r="B68" s="14"/>
+      <c r="C68" s="10"/>
+      <c r="D68" s="10"/>
+      <c r="E68" s="10"/>
+      <c r="F68" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G68" s="10"/>
+      <c r="H68" s="10"/>
+      <c r="I68" s="15"/>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A69" s="10"/>
+      <c r="B69" s="14"/>
+      <c r="C69" s="10"/>
+      <c r="D69" s="10"/>
+      <c r="E69" s="10"/>
+      <c r="F69" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G69" s="10"/>
+      <c r="H69" s="10"/>
+      <c r="I69" s="15"/>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A70" s="10"/>
+      <c r="B70" s="14"/>
+      <c r="C70" s="10"/>
+      <c r="D70" s="10"/>
+      <c r="E70" s="10"/>
+      <c r="F70" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="G70" s="10"/>
+      <c r="H70" s="10"/>
+      <c r="I70" s="15"/>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A71" s="10"/>
+      <c r="B71" s="14"/>
+      <c r="C71" s="10"/>
+      <c r="D71" s="10"/>
+      <c r="E71" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F71" s="10"/>
+      <c r="G71" s="10"/>
+      <c r="H71" s="10"/>
+      <c r="I71" s="15"/>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A72" s="10"/>
+      <c r="B72" s="14"/>
+      <c r="C72" s="10"/>
+      <c r="D72" s="10"/>
+      <c r="E72" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F72" s="10"/>
+      <c r="G72" s="10"/>
+      <c r="H72" s="10"/>
+      <c r="I72" s="15"/>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A73" s="10"/>
+      <c r="B73" s="14"/>
+      <c r="C73" s="10"/>
+      <c r="D73" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E73" s="10"/>
+      <c r="F73" s="10"/>
+      <c r="G73" s="10"/>
+      <c r="H73" s="10"/>
+      <c r="I73" s="15"/>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A74" s="10"/>
+      <c r="B74" s="16"/>
+      <c r="C74" s="17"/>
+      <c r="D74" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="E74" s="17"/>
+      <c r="F74" s="17"/>
+      <c r="G74" s="17"/>
+      <c r="H74" s="17"/>
+      <c r="I74" s="18"/>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B78" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C78" s="2"/>
+      <c r="D78" s="2"/>
+      <c r="E78" s="2"/>
+      <c r="F78" s="2"/>
+      <c r="G78" s="2"/>
+      <c r="H78" s="2"/>
+      <c r="I78" s="2"/>
+      <c r="J78" s="2"/>
+      <c r="K78" s="3"/>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B79" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C79" s="19"/>
+      <c r="D79" s="19"/>
+      <c r="E79" s="19"/>
+      <c r="F79" s="19"/>
+      <c r="G79" s="19"/>
+      <c r="H79" s="19"/>
+      <c r="I79" s="19"/>
+      <c r="J79" s="19"/>
+      <c r="K79" s="5"/>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B80" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C80" s="19"/>
+      <c r="D80" s="19"/>
+      <c r="E80" s="19"/>
+      <c r="F80" s="19"/>
+      <c r="G80" s="19"/>
+      <c r="H80" s="19"/>
+      <c r="I80" s="19"/>
+      <c r="J80" s="19"/>
+      <c r="K80" s="5"/>
+    </row>
+    <row r="81" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B81" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C81" s="19"/>
+      <c r="D81" s="19"/>
+      <c r="E81" s="19"/>
+      <c r="F81" s="19"/>
+      <c r="G81" s="19"/>
+      <c r="H81" s="19"/>
+      <c r="I81" s="19"/>
+      <c r="J81" s="19"/>
+      <c r="K81" s="5"/>
+    </row>
+    <row r="82" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B82" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C82" s="19"/>
+      <c r="D82" s="19"/>
+      <c r="E82" s="19"/>
+      <c r="F82" s="19"/>
+      <c r="G82" s="19"/>
+      <c r="H82" s="19"/>
+      <c r="I82" s="19"/>
+      <c r="J82" s="19"/>
+      <c r="K82" s="5"/>
+    </row>
+    <row r="83" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B83" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C83" s="19"/>
+      <c r="D83" s="19"/>
+      <c r="E83" s="19"/>
+      <c r="F83" s="19"/>
+      <c r="G83" s="19"/>
+      <c r="H83" s="19"/>
+      <c r="I83" s="19"/>
+      <c r="J83" s="19"/>
+      <c r="K83" s="5"/>
+    </row>
+    <row r="84" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B84" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C84" s="19"/>
+      <c r="D84" s="19"/>
+      <c r="E84" s="19"/>
+      <c r="F84" s="19"/>
+      <c r="G84" s="19"/>
+      <c r="H84" s="19"/>
+      <c r="I84" s="19"/>
+      <c r="J84" s="19"/>
+      <c r="K84" s="5"/>
+    </row>
+    <row r="85" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B85" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C85" s="19"/>
+      <c r="D85" s="19"/>
+      <c r="E85" s="19"/>
+      <c r="F85" s="19"/>
+      <c r="G85" s="19"/>
+      <c r="H85" s="19"/>
+      <c r="I85" s="19"/>
+      <c r="J85" s="19"/>
+      <c r="K85" s="5"/>
+    </row>
+    <row r="86" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B86" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C86" s="19"/>
+      <c r="D86" s="19"/>
+      <c r="E86" s="19"/>
+      <c r="F86" s="19"/>
+      <c r="G86" s="19"/>
+      <c r="H86" s="19"/>
+      <c r="I86" s="19"/>
+      <c r="J86" s="19"/>
+      <c r="K86" s="5"/>
+    </row>
+    <row r="87" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B87" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C87" s="19"/>
+      <c r="D87" s="19"/>
+      <c r="E87" s="19"/>
+      <c r="F87" s="19"/>
+      <c r="G87" s="19"/>
+      <c r="H87" s="19"/>
+      <c r="I87" s="19"/>
+      <c r="J87" s="19"/>
+      <c r="K87" s="5"/>
+    </row>
+    <row r="88" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B88" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C88" s="19"/>
+      <c r="D88" s="19"/>
+      <c r="E88" s="19"/>
+      <c r="F88" s="19"/>
+      <c r="G88" s="19"/>
+      <c r="H88" s="19"/>
+      <c r="I88" s="19"/>
+      <c r="J88" s="19"/>
+      <c r="K88" s="5"/>
+    </row>
+    <row r="89" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B89" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C89" s="19"/>
+      <c r="D89" s="19"/>
+      <c r="E89" s="19"/>
+      <c r="F89" s="19"/>
+      <c r="G89" s="19"/>
+      <c r="H89" s="19"/>
+      <c r="I89" s="19"/>
+      <c r="J89" s="19"/>
+      <c r="K89" s="5"/>
+    </row>
+    <row r="90" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B90" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C90" s="19"/>
+      <c r="D90" s="19"/>
+      <c r="E90" s="19"/>
+      <c r="F90" s="19"/>
+      <c r="G90" s="19"/>
+      <c r="H90" s="19"/>
+      <c r="I90" s="19"/>
+      <c r="J90" s="19"/>
+      <c r="K90" s="5"/>
+    </row>
+    <row r="91" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B91" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C91" s="19"/>
+      <c r="D91" s="19"/>
+      <c r="E91" s="19"/>
+      <c r="F91" s="19"/>
+      <c r="G91" s="19"/>
+      <c r="H91" s="19"/>
+      <c r="I91" s="19"/>
+      <c r="J91" s="19"/>
+      <c r="K91" s="5"/>
+    </row>
+    <row r="92" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B92" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C92" s="19"/>
+      <c r="D92" s="19"/>
+      <c r="E92" s="19"/>
+      <c r="F92" s="19"/>
+      <c r="G92" s="19"/>
+      <c r="H92" s="19"/>
+      <c r="I92" s="19"/>
+      <c r="J92" s="19"/>
+      <c r="K92" s="5"/>
+    </row>
+    <row r="93" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B93" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C93" s="19"/>
+      <c r="D93" s="19"/>
+      <c r="E93" s="19"/>
+      <c r="F93" s="19"/>
+      <c r="G93" s="19"/>
+      <c r="H93" s="19"/>
+      <c r="I93" s="19"/>
+      <c r="J93" s="19"/>
+      <c r="K93" s="5"/>
+    </row>
+    <row r="94" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B94" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C94" s="19"/>
+      <c r="D94" s="19"/>
+      <c r="E94" s="19"/>
+      <c r="F94" s="19"/>
+      <c r="G94" s="19"/>
+      <c r="H94" s="19"/>
+      <c r="I94" s="19"/>
+      <c r="J94" s="19"/>
+      <c r="K94" s="5"/>
+    </row>
+    <row r="95" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B95" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C95" s="19"/>
+      <c r="D95" s="19"/>
+      <c r="E95" s="19"/>
+      <c r="F95" s="19"/>
+      <c r="G95" s="19"/>
+      <c r="H95" s="19"/>
+      <c r="I95" s="19"/>
+      <c r="J95" s="19"/>
+      <c r="K95" s="5"/>
+    </row>
+    <row r="96" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B96" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C96" s="19"/>
+      <c r="D96" s="19"/>
+      <c r="E96" s="19"/>
+      <c r="F96" s="19"/>
+      <c r="G96" s="19"/>
+      <c r="H96" s="19"/>
+      <c r="I96" s="19"/>
+      <c r="J96" s="19"/>
+      <c r="K96" s="5"/>
+    </row>
+    <row r="97" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B97" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C97" s="19"/>
+      <c r="D97" s="19"/>
+      <c r="E97" s="19"/>
+      <c r="F97" s="19"/>
+      <c r="G97" s="19"/>
+      <c r="H97" s="19"/>
+      <c r="I97" s="19"/>
+      <c r="J97" s="19"/>
+      <c r="K97" s="5"/>
+    </row>
+    <row r="98" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B98" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C98" s="19"/>
+      <c r="D98" s="19"/>
+      <c r="E98" s="19"/>
+      <c r="F98" s="19"/>
+      <c r="G98" s="19"/>
+      <c r="H98" s="19"/>
+      <c r="I98" s="19"/>
+      <c r="J98" s="19"/>
+      <c r="K98" s="5"/>
+    </row>
+    <row r="99" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B99" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C99" s="19"/>
+      <c r="D99" s="19"/>
+      <c r="E99" s="19"/>
+      <c r="F99" s="19"/>
+      <c r="G99" s="19"/>
+      <c r="H99" s="19"/>
+      <c r="I99" s="19"/>
+      <c r="J99" s="19"/>
+      <c r="K99" s="5"/>
+    </row>
+    <row r="100" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B100" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C100" s="19"/>
+      <c r="D100" s="19"/>
+      <c r="E100" s="19"/>
+      <c r="F100" s="19"/>
+      <c r="G100" s="19"/>
+      <c r="H100" s="19"/>
+      <c r="I100" s="19"/>
+      <c r="J100" s="19"/>
+      <c r="K100" s="5"/>
+    </row>
+    <row r="101" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B101" s="4"/>
+      <c r="C101" s="19"/>
+      <c r="D101" s="19"/>
+      <c r="E101" s="19"/>
+      <c r="F101" s="19"/>
+      <c r="G101" s="19"/>
+      <c r="H101" s="19"/>
+      <c r="I101" s="19"/>
+      <c r="J101" s="19"/>
+      <c r="K101" s="5"/>
+    </row>
+    <row r="102" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B102" s="20" t="s">
+        <v>388</v>
+      </c>
+      <c r="C102" s="19"/>
+      <c r="D102" s="19"/>
+      <c r="E102" s="19"/>
+      <c r="F102" s="19"/>
+      <c r="G102" s="19"/>
+      <c r="H102" s="19"/>
+      <c r="I102" s="19"/>
+      <c r="J102" s="19"/>
+      <c r="K102" s="5"/>
+    </row>
+    <row r="103" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B103" s="20" t="s">
+        <v>389</v>
+      </c>
+      <c r="C103" s="19"/>
+      <c r="D103" s="19"/>
+      <c r="E103" s="19"/>
+      <c r="F103" s="19"/>
+      <c r="G103" s="19"/>
+      <c r="H103" s="19"/>
+      <c r="I103" s="19"/>
+      <c r="J103" s="19"/>
+      <c r="K103" s="5"/>
+    </row>
+    <row r="104" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B104" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="C104" s="19"/>
+      <c r="D104" s="19"/>
+      <c r="E104" s="19"/>
+      <c r="F104" s="19"/>
+      <c r="G104" s="19"/>
+      <c r="H104" s="19"/>
+      <c r="I104" s="19"/>
+      <c r="J104" s="19"/>
+      <c r="K104" s="5"/>
+    </row>
+    <row r="105" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B105" s="20" t="s">
+        <v>390</v>
+      </c>
+      <c r="C105" s="19"/>
+      <c r="D105" s="19"/>
+      <c r="E105" s="19"/>
+      <c r="F105" s="19"/>
+      <c r="G105" s="19"/>
+      <c r="H105" s="19"/>
+      <c r="I105" s="19"/>
+      <c r="J105" s="19"/>
+      <c r="K105" s="5"/>
+    </row>
+    <row r="106" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B106" s="20" t="s">
+        <v>391</v>
+      </c>
+      <c r="C106" s="19"/>
+      <c r="D106" s="19"/>
+      <c r="E106" s="19"/>
+      <c r="F106" s="19"/>
+      <c r="G106" s="19"/>
+      <c r="H106" s="19"/>
+      <c r="I106" s="19"/>
+      <c r="J106" s="19"/>
+      <c r="K106" s="5"/>
+    </row>
+    <row r="107" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B107" s="20" t="s">
+        <v>392</v>
+      </c>
+      <c r="C107" s="19"/>
+      <c r="D107" s="19"/>
+      <c r="E107" s="19"/>
+      <c r="F107" s="19"/>
+      <c r="G107" s="19"/>
+      <c r="H107" s="19"/>
+      <c r="I107" s="19"/>
+      <c r="J107" s="19"/>
+      <c r="K107" s="5"/>
+    </row>
+    <row r="108" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B108" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="C108" s="19"/>
+      <c r="D108" s="19"/>
+      <c r="E108" s="19"/>
+      <c r="F108" s="19"/>
+      <c r="G108" s="19"/>
+      <c r="H108" s="19"/>
+      <c r="I108" s="19"/>
+      <c r="J108" s="19"/>
+      <c r="K108" s="5"/>
+    </row>
+    <row r="109" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B109" s="20" t="s">
+        <v>221</v>
+      </c>
+      <c r="C109" s="19"/>
+      <c r="D109" s="19"/>
+      <c r="E109" s="19"/>
+      <c r="F109" s="19"/>
+      <c r="G109" s="19"/>
+      <c r="H109" s="19"/>
+      <c r="I109" s="19"/>
+      <c r="J109" s="19"/>
+      <c r="K109" s="5"/>
+    </row>
+    <row r="110" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B110" s="20" t="s">
+        <v>393</v>
+      </c>
+      <c r="C110" s="19"/>
+      <c r="D110" s="19"/>
+      <c r="E110" s="19"/>
+      <c r="F110" s="19"/>
+      <c r="G110" s="19"/>
+      <c r="H110" s="19"/>
+      <c r="I110" s="19"/>
+      <c r="J110" s="19"/>
+      <c r="K110" s="5"/>
+    </row>
+    <row r="111" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B111" s="20" t="s">
+        <v>394</v>
+      </c>
+      <c r="C111" s="19"/>
+      <c r="D111" s="19"/>
+      <c r="E111" s="19"/>
+      <c r="F111" s="19"/>
+      <c r="G111" s="19"/>
+      <c r="H111" s="19"/>
+      <c r="I111" s="19"/>
+      <c r="J111" s="19"/>
+      <c r="K111" s="5"/>
+    </row>
+    <row r="112" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B112" s="20" t="s">
+        <v>395</v>
+      </c>
+      <c r="C112" s="19"/>
+      <c r="D112" s="19"/>
+      <c r="E112" s="19"/>
+      <c r="F112" s="19"/>
+      <c r="G112" s="19"/>
+      <c r="H112" s="19"/>
+      <c r="I112" s="19"/>
+      <c r="J112" s="19"/>
+      <c r="K112" s="5"/>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B113" s="20" t="s">
+        <v>396</v>
+      </c>
+      <c r="C113" s="19"/>
+      <c r="D113" s="19"/>
+      <c r="E113" s="19"/>
+      <c r="F113" s="19"/>
+      <c r="G113" s="19"/>
+      <c r="H113" s="19"/>
+      <c r="I113" s="19"/>
+      <c r="J113" s="19"/>
+      <c r="K113" s="5"/>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B114" s="20" t="s">
+        <v>397</v>
+      </c>
+      <c r="C114" s="19"/>
+      <c r="D114" s="19"/>
+      <c r="E114" s="19"/>
+      <c r="F114" s="19"/>
+      <c r="G114" s="19"/>
+      <c r="H114" s="19"/>
+      <c r="I114" s="19"/>
+      <c r="J114" s="19"/>
+      <c r="K114" s="5"/>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B115" s="20" t="s">
+        <v>398</v>
+      </c>
+      <c r="C115" s="19"/>
+      <c r="D115" s="19"/>
+      <c r="E115" s="19"/>
+      <c r="F115" s="19"/>
+      <c r="G115" s="19"/>
+      <c r="H115" s="19"/>
+      <c r="I115" s="19"/>
+      <c r="J115" s="19"/>
+      <c r="K115" s="5"/>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B116" s="20" t="s">
+        <v>399</v>
+      </c>
+      <c r="C116" s="19"/>
+      <c r="D116" s="19"/>
+      <c r="E116" s="19"/>
+      <c r="F116" s="19"/>
+      <c r="G116" s="19"/>
+      <c r="H116" s="19"/>
+      <c r="I116" s="19"/>
+      <c r="J116" s="19"/>
+      <c r="K116" s="5"/>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B117" s="20" t="s">
+        <v>400</v>
+      </c>
+      <c r="C117" s="19"/>
+      <c r="D117" s="19"/>
+      <c r="E117" s="19"/>
+      <c r="F117" s="19"/>
+      <c r="G117" s="19"/>
+      <c r="H117" s="19"/>
+      <c r="I117" s="19"/>
+      <c r="J117" s="19"/>
+      <c r="K117" s="5"/>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B118" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="C118" s="19"/>
+      <c r="D118" s="19"/>
+      <c r="E118" s="19"/>
+      <c r="F118" s="19"/>
+      <c r="G118" s="19"/>
+      <c r="H118" s="19"/>
+      <c r="I118" s="19"/>
+      <c r="J118" s="19"/>
+      <c r="K118" s="5"/>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B119" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="C119" s="19"/>
+      <c r="D119" s="19"/>
+      <c r="E119" s="19"/>
+      <c r="F119" s="19"/>
+      <c r="G119" s="19"/>
+      <c r="H119" s="19"/>
+      <c r="I119" s="19"/>
+      <c r="J119" s="19"/>
+      <c r="K119" s="5"/>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B120" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="C120" s="19"/>
+      <c r="D120" s="19"/>
+      <c r="E120" s="19"/>
+      <c r="F120" s="19"/>
+      <c r="G120" s="19"/>
+      <c r="H120" s="19"/>
+      <c r="I120" s="19"/>
+      <c r="J120" s="19"/>
+      <c r="K120" s="5"/>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B121" s="20" t="s">
+        <v>401</v>
+      </c>
+      <c r="C121" s="19"/>
+      <c r="D121" s="19"/>
+      <c r="E121" s="19"/>
+      <c r="F121" s="19"/>
+      <c r="G121" s="19"/>
+      <c r="H121" s="19"/>
+      <c r="I121" s="19"/>
+      <c r="J121" s="19"/>
+      <c r="K121" s="5"/>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B122" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C122" s="8"/>
+      <c r="D122" s="8"/>
+      <c r="E122" s="8"/>
+      <c r="F122" s="8"/>
+      <c r="G122" s="8"/>
+      <c r="H122" s="8"/>
+      <c r="I122" s="8"/>
+      <c r="J122" s="8"/>
+      <c r="K122" s="9"/>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B126" s="21" t="s">
+        <v>403</v>
+      </c>
+      <c r="C126" s="22"/>
+      <c r="D126" s="22"/>
+      <c r="E126" s="22"/>
+      <c r="F126" s="22"/>
+      <c r="G126" s="22"/>
+      <c r="H126" s="23"/>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B127" s="20"/>
+      <c r="C127" s="24"/>
+      <c r="D127" s="24"/>
+      <c r="E127" s="24"/>
+      <c r="F127" s="24"/>
+      <c r="G127" s="24"/>
+      <c r="H127" s="25"/>
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B128" s="20" t="s">
+        <v>404</v>
+      </c>
+      <c r="C128" s="24"/>
+      <c r="D128" s="24"/>
+      <c r="E128" s="24"/>
+      <c r="F128" s="24"/>
+      <c r="G128" s="24"/>
+      <c r="H128" s="25"/>
+    </row>
+    <row r="129" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B129" s="20" t="s">
+        <v>405</v>
+      </c>
+      <c r="C129" s="24"/>
+      <c r="D129" s="24"/>
+      <c r="E129" s="24"/>
+      <c r="F129" s="24"/>
+      <c r="G129" s="24"/>
+      <c r="H129" s="25"/>
+    </row>
+    <row r="130" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B130" s="20"/>
+      <c r="C130" s="24"/>
+      <c r="D130" s="24"/>
+      <c r="E130" s="24"/>
+      <c r="F130" s="24"/>
+      <c r="G130" s="24"/>
+      <c r="H130" s="25"/>
+    </row>
+    <row r="131" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B131" s="21" t="s">
+        <v>406</v>
+      </c>
+      <c r="C131" s="22"/>
+      <c r="D131" s="22"/>
+      <c r="E131" s="22"/>
+      <c r="F131" s="22"/>
+      <c r="G131" s="22"/>
+      <c r="H131" s="23"/>
+    </row>
+    <row r="132" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B132" s="20" t="s">
+        <v>407</v>
+      </c>
+      <c r="C132" s="24"/>
+      <c r="D132" s="24"/>
+      <c r="E132" s="24"/>
+      <c r="F132" s="24"/>
+      <c r="G132" s="24"/>
+      <c r="H132" s="25"/>
+    </row>
+    <row r="133" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B133" s="20" t="s">
+        <v>408</v>
+      </c>
+      <c r="C133" s="24"/>
+      <c r="D133" s="24"/>
+      <c r="E133" s="24"/>
+      <c r="F133" s="24"/>
+      <c r="G133" s="24"/>
+      <c r="H133" s="25"/>
+    </row>
+    <row r="134" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B134" s="20" t="s">
+        <v>409</v>
+      </c>
+      <c r="C134" s="24"/>
+      <c r="D134" s="24"/>
+      <c r="E134" s="24"/>
+      <c r="F134" s="24"/>
+      <c r="G134" s="24"/>
+      <c r="H134" s="25"/>
+    </row>
+    <row r="135" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B135" s="20" t="s">
+        <v>189</v>
+      </c>
+      <c r="C135" s="24"/>
+      <c r="D135" s="24"/>
+      <c r="E135" s="24"/>
+      <c r="F135" s="24"/>
+      <c r="G135" s="24"/>
+      <c r="H135" s="25"/>
+    </row>
+    <row r="136" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B136" s="20" t="s">
+        <v>410</v>
+      </c>
+      <c r="C136" s="24"/>
+      <c r="D136" s="24"/>
+      <c r="E136" s="24"/>
+      <c r="F136" s="24"/>
+      <c r="G136" s="24"/>
+      <c r="H136" s="25"/>
+    </row>
+    <row r="137" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B137" s="20" t="s">
+        <v>249</v>
+      </c>
+      <c r="C137" s="24"/>
+      <c r="D137" s="24"/>
+      <c r="E137" s="24"/>
+      <c r="F137" s="24"/>
+      <c r="G137" s="24"/>
+      <c r="H137" s="25"/>
+    </row>
+    <row r="138" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B138" s="20" t="s">
+        <v>411</v>
+      </c>
+      <c r="C138" s="24"/>
+      <c r="D138" s="24"/>
+      <c r="E138" s="24"/>
+      <c r="F138" s="24"/>
+      <c r="G138" s="24"/>
+      <c r="H138" s="25"/>
+    </row>
+    <row r="139" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B139" s="20" t="s">
+        <v>412</v>
+      </c>
+      <c r="C139" s="24"/>
+      <c r="D139" s="24"/>
+      <c r="E139" s="24"/>
+      <c r="F139" s="24"/>
+      <c r="G139" s="24"/>
+      <c r="H139" s="25"/>
+    </row>
+    <row r="140" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B140" s="20" t="s">
+        <v>413</v>
+      </c>
+      <c r="C140" s="24"/>
+      <c r="D140" s="24"/>
+      <c r="E140" s="24"/>
+      <c r="F140" s="24"/>
+      <c r="G140" s="24"/>
+      <c r="H140" s="25"/>
+    </row>
+    <row r="141" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B141" s="20" t="s">
+        <v>339</v>
+      </c>
+      <c r="C141" s="24"/>
+      <c r="D141" s="24"/>
+      <c r="E141" s="24"/>
+      <c r="F141" s="24"/>
+      <c r="G141" s="24"/>
+      <c r="H141" s="25"/>
+    </row>
+    <row r="142" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B142" s="20"/>
+      <c r="C142" s="24"/>
+      <c r="D142" s="24"/>
+      <c r="E142" s="24"/>
+      <c r="F142" s="24"/>
+      <c r="G142" s="24"/>
+      <c r="H142" s="25"/>
+    </row>
+    <row r="143" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B143" s="20" t="s">
+        <v>414</v>
+      </c>
+      <c r="C143" s="24"/>
+      <c r="D143" s="24"/>
+      <c r="E143" s="24"/>
+      <c r="F143" s="24"/>
+      <c r="G143" s="24"/>
+      <c r="H143" s="25"/>
+    </row>
+    <row r="144" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B144" s="20" t="s">
+        <v>415</v>
+      </c>
+      <c r="C144" s="24"/>
+      <c r="D144" s="24"/>
+      <c r="E144" s="24"/>
+      <c r="F144" s="24"/>
+      <c r="G144" s="24"/>
+      <c r="H144" s="25"/>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B145" s="20" t="s">
+        <v>339</v>
+      </c>
+      <c r="C145" s="24"/>
+      <c r="D145" s="24"/>
+      <c r="E145" s="24"/>
+      <c r="F145" s="24"/>
+      <c r="G145" s="24"/>
+      <c r="H145" s="25"/>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B146" s="20" t="s">
+        <v>192</v>
+      </c>
+      <c r="C146" s="24"/>
+      <c r="D146" s="24"/>
+      <c r="E146" s="24"/>
+      <c r="F146" s="24"/>
+      <c r="G146" s="24"/>
+      <c r="H146" s="25"/>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B147" s="20" t="s">
+        <v>193</v>
+      </c>
+      <c r="C147" s="24"/>
+      <c r="D147" s="24"/>
+      <c r="E147" s="24"/>
+      <c r="F147" s="24"/>
+      <c r="G147" s="24"/>
+      <c r="H147" s="25"/>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B148" s="20" t="s">
+        <v>194</v>
+      </c>
+      <c r="C148" s="24"/>
+      <c r="D148" s="24"/>
+      <c r="E148" s="24"/>
+      <c r="F148" s="24"/>
+      <c r="G148" s="24"/>
+      <c r="H148" s="25"/>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B149" s="26" t="s">
+        <v>207</v>
+      </c>
+      <c r="C149" s="27"/>
+      <c r="D149" s="27"/>
+      <c r="E149" s="27"/>
+      <c r="F149" s="27"/>
+      <c r="G149" s="27"/>
+      <c r="H149" s="28"/>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B150" s="20"/>
+      <c r="C150" s="24"/>
+      <c r="D150" s="24"/>
+      <c r="E150" s="24"/>
+      <c r="F150" s="24"/>
+      <c r="G150" s="24"/>
+      <c r="H150" s="25"/>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B151" s="20" t="s">
+        <v>416</v>
+      </c>
+      <c r="C151" s="24"/>
+      <c r="D151" s="24"/>
+      <c r="E151" s="24"/>
+      <c r="F151" s="24"/>
+      <c r="G151" s="24"/>
+      <c r="H151" s="25"/>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B152" s="20" t="s">
+        <v>417</v>
+      </c>
+      <c r="C152" s="24"/>
+      <c r="D152" s="24"/>
+      <c r="E152" s="24"/>
+      <c r="F152" s="24"/>
+      <c r="G152" s="24"/>
+      <c r="H152" s="25"/>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B153" s="20" t="s">
+        <v>418</v>
+      </c>
+      <c r="C153" s="24"/>
+      <c r="D153" s="24"/>
+      <c r="E153" s="24"/>
+      <c r="F153" s="24"/>
+      <c r="G153" s="24"/>
+      <c r="H153" s="25"/>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B154" s="20" t="s">
+        <v>419</v>
+      </c>
+      <c r="C154" s="24"/>
+      <c r="D154" s="24"/>
+      <c r="E154" s="24"/>
+      <c r="F154" s="24"/>
+      <c r="G154" s="24"/>
+      <c r="H154" s="25"/>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B155" s="20" t="s">
+        <v>194</v>
+      </c>
+      <c r="C155" s="24"/>
+      <c r="D155" s="24"/>
+      <c r="E155" s="24"/>
+      <c r="F155" s="24"/>
+      <c r="G155" s="24"/>
+      <c r="H155" s="25"/>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B156" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="C156" s="24"/>
+      <c r="D156" s="24"/>
+      <c r="E156" s="24"/>
+      <c r="F156" s="24"/>
+      <c r="G156" s="24"/>
+      <c r="H156" s="25"/>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B157" s="26" t="s">
+        <v>208</v>
+      </c>
+      <c r="C157" s="27"/>
+      <c r="D157" s="27"/>
+      <c r="E157" s="27"/>
+      <c r="F157" s="27"/>
+      <c r="G157" s="27"/>
+      <c r="H157" s="28"/>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B161" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C161" s="2"/>
+      <c r="D161" s="2"/>
+      <c r="E161" s="3"/>
+    </row>
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B162" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="C162" s="19"/>
+      <c r="D162" s="19"/>
+      <c r="E162" s="5"/>
+    </row>
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B163" s="20" t="s">
+        <v>420</v>
+      </c>
+      <c r="C163" s="19"/>
+      <c r="D163" s="19"/>
+      <c r="E163" s="5"/>
+    </row>
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B164" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="C164" s="8"/>
+      <c r="D164" s="8"/>
+      <c r="E164" s="9"/>
+    </row>
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B168" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="C168" s="2"/>
+      <c r="D168" s="2"/>
+      <c r="E168" s="2"/>
+      <c r="F168" s="2"/>
+      <c r="G168" s="2"/>
+      <c r="H168" s="2"/>
+      <c r="I168" s="2"/>
+      <c r="J168" s="3"/>
+    </row>
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B169" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="C169" s="19"/>
+      <c r="D169" s="19"/>
+      <c r="E169" s="19"/>
+      <c r="F169" s="19"/>
+      <c r="G169" s="19"/>
+      <c r="H169" s="19"/>
+      <c r="I169" s="19"/>
+      <c r="J169" s="5"/>
+    </row>
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B170" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="C170" s="19"/>
+      <c r="D170" s="19"/>
+      <c r="E170" s="19"/>
+      <c r="F170" s="19"/>
+      <c r="G170" s="19"/>
+      <c r="H170" s="19"/>
+      <c r="I170" s="19"/>
+      <c r="J170" s="5"/>
+    </row>
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B171" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="C171" s="19"/>
+      <c r="D171" s="19"/>
+      <c r="E171" s="19"/>
+      <c r="F171" s="19"/>
+      <c r="G171" s="19"/>
+      <c r="H171" s="19"/>
+      <c r="I171" s="19"/>
+      <c r="J171" s="5"/>
+    </row>
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B172" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="C172" s="19"/>
+      <c r="D172" s="19"/>
+      <c r="E172" s="19"/>
+      <c r="F172" s="19"/>
+      <c r="G172" s="19"/>
+      <c r="H172" s="19"/>
+      <c r="I172" s="19"/>
+      <c r="J172" s="5"/>
+    </row>
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B173" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="C173" s="19"/>
+      <c r="D173" s="19"/>
+      <c r="E173" s="19"/>
+      <c r="F173" s="19"/>
+      <c r="G173" s="19"/>
+      <c r="H173" s="19"/>
+      <c r="I173" s="19"/>
+      <c r="J173" s="5"/>
+    </row>
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B174" s="4"/>
+      <c r="C174" s="19"/>
+      <c r="D174" s="19"/>
+      <c r="E174" s="19"/>
+      <c r="F174" s="19"/>
+      <c r="G174" s="19"/>
+      <c r="H174" s="19"/>
+      <c r="I174" s="19"/>
+      <c r="J174" s="5"/>
+    </row>
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B175" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="C175" s="19"/>
+      <c r="D175" s="19"/>
+      <c r="E175" s="19"/>
+      <c r="F175" s="19"/>
+      <c r="G175" s="19"/>
+      <c r="H175" s="19"/>
+      <c r="I175" s="19"/>
+      <c r="J175" s="5"/>
+    </row>
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B176" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="C176" s="19"/>
+      <c r="D176" s="19"/>
+      <c r="E176" s="19"/>
+      <c r="F176" s="19"/>
+      <c r="G176" s="19"/>
+      <c r="H176" s="19"/>
+      <c r="I176" s="19"/>
+      <c r="J176" s="5"/>
+    </row>
+    <row r="177" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B177" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="C177" s="19"/>
+      <c r="D177" s="19"/>
+      <c r="E177" s="19"/>
+      <c r="F177" s="19"/>
+      <c r="G177" s="19"/>
+      <c r="H177" s="19"/>
+      <c r="I177" s="19"/>
+      <c r="J177" s="5"/>
+    </row>
+    <row r="178" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B178" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="C178" s="19"/>
+      <c r="D178" s="19"/>
+      <c r="E178" s="19"/>
+      <c r="F178" s="19"/>
+      <c r="G178" s="19"/>
+      <c r="H178" s="19"/>
+      <c r="I178" s="19"/>
+      <c r="J178" s="5"/>
+    </row>
+    <row r="179" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B179" s="4"/>
+      <c r="C179" s="19"/>
+      <c r="D179" s="19"/>
+      <c r="E179" s="19"/>
+      <c r="F179" s="19"/>
+      <c r="G179" s="19"/>
+      <c r="H179" s="19"/>
+      <c r="I179" s="19"/>
+      <c r="J179" s="5"/>
+    </row>
+    <row r="180" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B180" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="C180" s="19"/>
+      <c r="D180" s="19"/>
+      <c r="E180" s="19"/>
+      <c r="F180" s="19"/>
+      <c r="G180" s="19"/>
+      <c r="H180" s="19"/>
+      <c r="I180" s="19"/>
+      <c r="J180" s="5"/>
+    </row>
+    <row r="181" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B181" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="C181" s="19"/>
+      <c r="D181" s="19"/>
+      <c r="E181" s="19"/>
+      <c r="F181" s="19"/>
+      <c r="G181" s="19"/>
+      <c r="H181" s="19"/>
+      <c r="I181" s="19"/>
+      <c r="J181" s="5"/>
+    </row>
+    <row r="182" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B182" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="C182" s="19"/>
+      <c r="D182" s="19"/>
+      <c r="E182" s="19"/>
+      <c r="F182" s="19"/>
+      <c r="G182" s="19"/>
+      <c r="H182" s="19"/>
+      <c r="I182" s="19"/>
+      <c r="J182" s="5"/>
+    </row>
+    <row r="183" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B183" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="C183" s="19"/>
+      <c r="D183" s="19"/>
+      <c r="E183" s="19"/>
+      <c r="F183" s="19"/>
+      <c r="G183" s="19"/>
+      <c r="H183" s="19"/>
+      <c r="I183" s="19"/>
+      <c r="J183" s="5"/>
+    </row>
+    <row r="184" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B184" s="4"/>
+      <c r="C184" s="19"/>
+      <c r="D184" s="19"/>
+      <c r="E184" s="19"/>
+      <c r="F184" s="19"/>
+      <c r="G184" s="19"/>
+      <c r="H184" s="19"/>
+      <c r="I184" s="19"/>
+      <c r="J184" s="5"/>
+    </row>
+    <row r="185" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B185" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="C185" s="19"/>
+      <c r="D185" s="19"/>
+      <c r="E185" s="19"/>
+      <c r="F185" s="19"/>
+      <c r="G185" s="19"/>
+      <c r="H185" s="19"/>
+      <c r="I185" s="19"/>
+      <c r="J185" s="5"/>
+    </row>
+    <row r="186" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B186" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="C186" s="19"/>
+      <c r="D186" s="19"/>
+      <c r="E186" s="19"/>
+      <c r="F186" s="19"/>
+      <c r="G186" s="19"/>
+      <c r="H186" s="19"/>
+      <c r="I186" s="19"/>
+      <c r="J186" s="5"/>
+    </row>
+    <row r="187" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B187" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="C187" s="19"/>
+      <c r="D187" s="19"/>
+      <c r="E187" s="19"/>
+      <c r="F187" s="19"/>
+      <c r="G187" s="19"/>
+      <c r="H187" s="19"/>
+      <c r="I187" s="19"/>
+      <c r="J187" s="5"/>
+    </row>
+    <row r="188" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B188" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="C188" s="19"/>
+      <c r="D188" s="19"/>
+      <c r="E188" s="19"/>
+      <c r="F188" s="19"/>
+      <c r="G188" s="19"/>
+      <c r="H188" s="19"/>
+      <c r="I188" s="19"/>
+      <c r="J188" s="5"/>
+    </row>
+    <row r="189" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B189" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="C189" s="19"/>
+      <c r="D189" s="19"/>
+      <c r="E189" s="19"/>
+      <c r="F189" s="19"/>
+      <c r="G189" s="19"/>
+      <c r="H189" s="19"/>
+      <c r="I189" s="19"/>
+      <c r="J189" s="5"/>
+    </row>
+    <row r="190" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B190" s="4"/>
+      <c r="C190" s="19"/>
+      <c r="D190" s="19"/>
+      <c r="E190" s="19"/>
+      <c r="F190" s="19"/>
+      <c r="G190" s="19"/>
+      <c r="H190" s="19"/>
+      <c r="I190" s="19"/>
+      <c r="J190" s="5"/>
+    </row>
+    <row r="191" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B191" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="C191" s="19"/>
+      <c r="D191" s="19"/>
+      <c r="E191" s="19"/>
+      <c r="F191" s="19"/>
+      <c r="G191" s="19"/>
+      <c r="H191" s="19"/>
+      <c r="I191" s="19"/>
+      <c r="J191" s="5"/>
+    </row>
+    <row r="192" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B192" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="C192" s="19"/>
+      <c r="D192" s="19"/>
+      <c r="E192" s="19"/>
+      <c r="F192" s="19"/>
+      <c r="G192" s="19"/>
+      <c r="H192" s="19"/>
+      <c r="I192" s="19"/>
+      <c r="J192" s="5"/>
+    </row>
+    <row r="193" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B193" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="C193" s="19"/>
+      <c r="D193" s="19"/>
+      <c r="E193" s="19"/>
+      <c r="F193" s="19"/>
+      <c r="G193" s="19"/>
+      <c r="H193" s="19"/>
+      <c r="I193" s="19"/>
+      <c r="J193" s="5"/>
+    </row>
+    <row r="194" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B194" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="C194" s="19"/>
+      <c r="D194" s="19"/>
+      <c r="E194" s="19"/>
+      <c r="F194" s="19"/>
+      <c r="G194" s="19"/>
+      <c r="H194" s="19"/>
+      <c r="I194" s="19"/>
+      <c r="J194" s="5"/>
+    </row>
+    <row r="195" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B195" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="C195" s="19"/>
+      <c r="D195" s="19"/>
+      <c r="E195" s="19"/>
+      <c r="F195" s="19"/>
+      <c r="G195" s="19"/>
+      <c r="H195" s="19"/>
+      <c r="I195" s="19"/>
+      <c r="J195" s="5"/>
+    </row>
+    <row r="196" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B196" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="C196" s="19"/>
+      <c r="D196" s="19"/>
+      <c r="E196" s="19"/>
+      <c r="F196" s="19"/>
+      <c r="G196" s="19"/>
+      <c r="H196" s="19"/>
+      <c r="I196" s="19"/>
+      <c r="J196" s="5"/>
+    </row>
+    <row r="197" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B197" s="4"/>
+      <c r="C197" s="19"/>
+      <c r="D197" s="19"/>
+      <c r="E197" s="19"/>
+      <c r="F197" s="19"/>
+      <c r="G197" s="19"/>
+      <c r="H197" s="19"/>
+      <c r="I197" s="19"/>
+      <c r="J197" s="5"/>
+    </row>
+    <row r="198" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B198" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="C198" s="19"/>
+      <c r="D198" s="19"/>
+      <c r="E198" s="19"/>
+      <c r="F198" s="19"/>
+      <c r="G198" s="19"/>
+      <c r="H198" s="19"/>
+      <c r="I198" s="19"/>
+      <c r="J198" s="5"/>
+    </row>
+    <row r="199" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B199" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="C199" s="19"/>
+      <c r="D199" s="19"/>
+      <c r="E199" s="19"/>
+      <c r="F199" s="19"/>
+      <c r="G199" s="19"/>
+      <c r="H199" s="19"/>
+      <c r="I199" s="19"/>
+      <c r="J199" s="5"/>
+    </row>
+    <row r="200" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B200" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="C200" s="19"/>
+      <c r="D200" s="19"/>
+      <c r="E200" s="19"/>
+      <c r="F200" s="19"/>
+      <c r="G200" s="19"/>
+      <c r="H200" s="19"/>
+      <c r="I200" s="19"/>
+      <c r="J200" s="5"/>
+    </row>
+    <row r="201" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B201" s="4"/>
+      <c r="C201" s="19"/>
+      <c r="D201" s="19"/>
+      <c r="E201" s="19"/>
+      <c r="F201" s="19"/>
+      <c r="G201" s="19"/>
+      <c r="H201" s="19"/>
+      <c r="I201" s="19"/>
+      <c r="J201" s="5"/>
+    </row>
+    <row r="202" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B202" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="C202" s="19"/>
+      <c r="D202" s="19"/>
+      <c r="E202" s="19"/>
+      <c r="F202" s="19"/>
+      <c r="G202" s="19"/>
+      <c r="H202" s="19"/>
+      <c r="I202" s="19"/>
+      <c r="J202" s="5"/>
+    </row>
+    <row r="203" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B203" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="C203" s="19"/>
+      <c r="D203" s="19"/>
+      <c r="E203" s="19"/>
+      <c r="F203" s="19"/>
+      <c r="G203" s="19"/>
+      <c r="H203" s="19"/>
+      <c r="I203" s="19"/>
+      <c r="J203" s="5"/>
+    </row>
+    <row r="204" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B204" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="C204" s="19"/>
+      <c r="D204" s="19"/>
+      <c r="E204" s="19"/>
+      <c r="F204" s="19"/>
+      <c r="G204" s="19"/>
+      <c r="H204" s="19"/>
+      <c r="I204" s="19"/>
+      <c r="J204" s="5"/>
+    </row>
+    <row r="205" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B205" s="4"/>
+      <c r="C205" s="19"/>
+      <c r="D205" s="19"/>
+      <c r="E205" s="19"/>
+      <c r="F205" s="19"/>
+      <c r="G205" s="19"/>
+      <c r="H205" s="19"/>
+      <c r="I205" s="19"/>
+      <c r="J205" s="5"/>
+    </row>
+    <row r="206" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B206" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="C206" s="19"/>
+      <c r="D206" s="19"/>
+      <c r="E206" s="19"/>
+      <c r="F206" s="19"/>
+      <c r="G206" s="19"/>
+      <c r="H206" s="19"/>
+      <c r="I206" s="19"/>
+      <c r="J206" s="5"/>
+    </row>
+    <row r="207" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B207" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="C207" s="19"/>
+      <c r="D207" s="19"/>
+      <c r="E207" s="19"/>
+      <c r="F207" s="19"/>
+      <c r="G207" s="19"/>
+      <c r="H207" s="19"/>
+      <c r="I207" s="19"/>
+      <c r="J207" s="5"/>
+    </row>
+    <row r="208" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B208" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="C208" s="19"/>
+      <c r="D208" s="19"/>
+      <c r="E208" s="19"/>
+      <c r="F208" s="19"/>
+      <c r="G208" s="19"/>
+      <c r="H208" s="19"/>
+      <c r="I208" s="19"/>
+      <c r="J208" s="5"/>
+    </row>
+    <row r="209" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B209" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="C209" s="19"/>
+      <c r="D209" s="19"/>
+      <c r="E209" s="19"/>
+      <c r="F209" s="19"/>
+      <c r="G209" s="19"/>
+      <c r="H209" s="19"/>
+      <c r="I209" s="19"/>
+      <c r="J209" s="5"/>
+    </row>
+    <row r="210" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B210" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="C210" s="19"/>
+      <c r="D210" s="19"/>
+      <c r="E210" s="19"/>
+      <c r="F210" s="19"/>
+      <c r="G210" s="19"/>
+      <c r="H210" s="19"/>
+      <c r="I210" s="19"/>
+      <c r="J210" s="5"/>
+    </row>
+    <row r="211" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B211" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="C211" s="19"/>
+      <c r="D211" s="19"/>
+      <c r="E211" s="19"/>
+      <c r="F211" s="19"/>
+      <c r="G211" s="19"/>
+      <c r="H211" s="19"/>
+      <c r="I211" s="19"/>
+      <c r="J211" s="5"/>
+    </row>
+    <row r="212" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B212" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="C212" s="19"/>
+      <c r="D212" s="19"/>
+      <c r="E212" s="19"/>
+      <c r="F212" s="19"/>
+      <c r="G212" s="19"/>
+      <c r="H212" s="19"/>
+      <c r="I212" s="19"/>
+      <c r="J212" s="5"/>
+    </row>
+    <row r="213" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B213" s="4" t="s">
+        <v>342</v>
+      </c>
+      <c r="C213" s="19"/>
+      <c r="D213" s="19"/>
+      <c r="E213" s="19"/>
+      <c r="F213" s="19"/>
+      <c r="G213" s="19"/>
+      <c r="H213" s="19"/>
+      <c r="I213" s="19"/>
+      <c r="J213" s="5"/>
+    </row>
+    <row r="214" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B214" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="C214" s="19"/>
+      <c r="D214" s="19"/>
+      <c r="E214" s="19"/>
+      <c r="F214" s="19"/>
+      <c r="G214" s="19"/>
+      <c r="H214" s="19"/>
+      <c r="I214" s="19"/>
+      <c r="J214" s="5"/>
+    </row>
+    <row r="215" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B215" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="C215" s="19"/>
+      <c r="D215" s="19"/>
+      <c r="E215" s="19"/>
+      <c r="F215" s="19"/>
+      <c r="G215" s="19"/>
+      <c r="H215" s="19"/>
+      <c r="I215" s="19"/>
+      <c r="J215" s="5"/>
+    </row>
+    <row r="216" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B216" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="C216" s="19"/>
+      <c r="D216" s="19"/>
+      <c r="E216" s="19"/>
+      <c r="F216" s="19"/>
+      <c r="G216" s="19"/>
+      <c r="H216" s="19"/>
+      <c r="I216" s="19"/>
+      <c r="J216" s="5"/>
+    </row>
+    <row r="217" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B217" s="4"/>
+      <c r="C217" s="19"/>
+      <c r="D217" s="19"/>
+      <c r="E217" s="19"/>
+      <c r="F217" s="19"/>
+      <c r="G217" s="19"/>
+      <c r="H217" s="19"/>
+      <c r="I217" s="19"/>
+      <c r="J217" s="5"/>
+    </row>
+    <row r="218" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B218" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="C218" s="19"/>
+      <c r="D218" s="19"/>
+      <c r="E218" s="19"/>
+      <c r="F218" s="19"/>
+      <c r="G218" s="19"/>
+      <c r="H218" s="19"/>
+      <c r="I218" s="19"/>
+      <c r="J218" s="5"/>
+    </row>
+    <row r="219" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B219" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="C219" s="19"/>
+      <c r="D219" s="19"/>
+      <c r="E219" s="19"/>
+      <c r="F219" s="19"/>
+      <c r="G219" s="19"/>
+      <c r="H219" s="19"/>
+      <c r="I219" s="19"/>
+      <c r="J219" s="5"/>
+    </row>
+    <row r="220" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B220" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="C220" s="19"/>
+      <c r="D220" s="19"/>
+      <c r="E220" s="19"/>
+      <c r="F220" s="19"/>
+      <c r="G220" s="19"/>
+      <c r="H220" s="19"/>
+      <c r="I220" s="19"/>
+      <c r="J220" s="5"/>
+    </row>
+    <row r="221" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B221" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="C221" s="19"/>
+      <c r="D221" s="19"/>
+      <c r="E221" s="19"/>
+      <c r="F221" s="19"/>
+      <c r="G221" s="19"/>
+      <c r="H221" s="19"/>
+      <c r="I221" s="19"/>
+      <c r="J221" s="5"/>
+    </row>
+    <row r="222" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B222" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="C222" s="19"/>
+      <c r="D222" s="19"/>
+      <c r="E222" s="19"/>
+      <c r="F222" s="19"/>
+      <c r="G222" s="19"/>
+      <c r="H222" s="19"/>
+      <c r="I222" s="19"/>
+      <c r="J222" s="5"/>
+    </row>
+    <row r="223" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B223" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="C223" s="19"/>
+      <c r="D223" s="19"/>
+      <c r="E223" s="19"/>
+      <c r="F223" s="19"/>
+      <c r="G223" s="19"/>
+      <c r="H223" s="19"/>
+      <c r="I223" s="19"/>
+      <c r="J223" s="5"/>
+    </row>
+    <row r="224" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B224" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="C224" s="19"/>
+      <c r="D224" s="19"/>
+      <c r="E224" s="19"/>
+      <c r="F224" s="19"/>
+      <c r="G224" s="19"/>
+      <c r="H224" s="19"/>
+      <c r="I224" s="19"/>
+      <c r="J224" s="5"/>
+    </row>
+    <row r="225" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B225" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="C225" s="19"/>
+      <c r="D225" s="19"/>
+      <c r="E225" s="19"/>
+      <c r="F225" s="19"/>
+      <c r="G225" s="19"/>
+      <c r="H225" s="19"/>
+      <c r="I225" s="19"/>
+      <c r="J225" s="5"/>
+    </row>
+    <row r="226" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B226" s="4"/>
+      <c r="C226" s="19"/>
+      <c r="D226" s="19"/>
+      <c r="E226" s="19"/>
+      <c r="F226" s="19"/>
+      <c r="G226" s="19"/>
+      <c r="H226" s="19"/>
+      <c r="I226" s="19"/>
+      <c r="J226" s="5"/>
+    </row>
+    <row r="227" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B227" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="C227" s="19"/>
+      <c r="D227" s="19"/>
+      <c r="E227" s="19"/>
+      <c r="F227" s="19"/>
+      <c r="G227" s="19"/>
+      <c r="H227" s="19"/>
+      <c r="I227" s="19"/>
+      <c r="J227" s="5"/>
+    </row>
+    <row r="228" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B228" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="C228" s="19"/>
+      <c r="D228" s="19"/>
+      <c r="E228" s="19"/>
+      <c r="F228" s="19"/>
+      <c r="G228" s="19"/>
+      <c r="H228" s="19"/>
+      <c r="I228" s="19"/>
+      <c r="J228" s="5"/>
+    </row>
+    <row r="229" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B229" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="C229" s="19"/>
+      <c r="D229" s="19"/>
+      <c r="E229" s="19"/>
+      <c r="F229" s="19"/>
+      <c r="G229" s="19"/>
+      <c r="H229" s="19"/>
+      <c r="I229" s="19"/>
+      <c r="J229" s="5"/>
+    </row>
+    <row r="230" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B230" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="C230" s="19"/>
+      <c r="D230" s="19"/>
+      <c r="E230" s="19"/>
+      <c r="F230" s="19"/>
+      <c r="G230" s="19"/>
+      <c r="H230" s="19"/>
+      <c r="I230" s="19"/>
+      <c r="J230" s="5"/>
+    </row>
+    <row r="231" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B231" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="C231" s="19"/>
+      <c r="D231" s="19"/>
+      <c r="E231" s="19"/>
+      <c r="F231" s="19"/>
+      <c r="G231" s="19"/>
+      <c r="H231" s="19"/>
+      <c r="I231" s="19"/>
+      <c r="J231" s="5"/>
+    </row>
+    <row r="232" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B232" s="4"/>
+      <c r="C232" s="19"/>
+      <c r="D232" s="19"/>
+      <c r="E232" s="19"/>
+      <c r="F232" s="19"/>
+      <c r="G232" s="19"/>
+      <c r="H232" s="19"/>
+      <c r="I232" s="19"/>
+      <c r="J232" s="5"/>
+    </row>
+    <row r="233" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B233" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="C233" s="19"/>
+      <c r="D233" s="19"/>
+      <c r="E233" s="19"/>
+      <c r="F233" s="19"/>
+      <c r="G233" s="19"/>
+      <c r="H233" s="19"/>
+      <c r="I233" s="19"/>
+      <c r="J233" s="5"/>
+    </row>
+    <row r="234" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B234" s="4" t="s">
+        <v>352</v>
+      </c>
+      <c r="C234" s="19"/>
+      <c r="D234" s="19"/>
+      <c r="E234" s="19"/>
+      <c r="F234" s="19"/>
+      <c r="G234" s="19"/>
+      <c r="H234" s="19"/>
+      <c r="I234" s="19"/>
+      <c r="J234" s="5"/>
+    </row>
+    <row r="235" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B235" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="C235" s="19"/>
+      <c r="D235" s="19"/>
+      <c r="E235" s="19"/>
+      <c r="F235" s="19"/>
+      <c r="G235" s="19"/>
+      <c r="H235" s="19"/>
+      <c r="I235" s="19"/>
+      <c r="J235" s="5"/>
+    </row>
+    <row r="236" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B236" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="C236" s="19"/>
+      <c r="D236" s="19"/>
+      <c r="E236" s="19"/>
+      <c r="F236" s="19"/>
+      <c r="G236" s="19"/>
+      <c r="H236" s="19"/>
+      <c r="I236" s="19"/>
+      <c r="J236" s="5"/>
+    </row>
+    <row r="237" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B237" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="C237" s="19"/>
+      <c r="D237" s="19"/>
+      <c r="E237" s="19"/>
+      <c r="F237" s="19"/>
+      <c r="G237" s="19"/>
+      <c r="H237" s="19"/>
+      <c r="I237" s="19"/>
+      <c r="J237" s="5"/>
+    </row>
+    <row r="238" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B238" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="C238" s="19"/>
+      <c r="D238" s="19"/>
+      <c r="E238" s="19"/>
+      <c r="F238" s="19"/>
+      <c r="G238" s="19"/>
+      <c r="H238" s="19"/>
+      <c r="I238" s="19"/>
+      <c r="J238" s="5"/>
+    </row>
+    <row r="239" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B239" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="C239" s="19"/>
+      <c r="D239" s="19"/>
+      <c r="E239" s="19"/>
+      <c r="F239" s="19"/>
+      <c r="G239" s="19"/>
+      <c r="H239" s="19"/>
+      <c r="I239" s="19"/>
+      <c r="J239" s="5"/>
+    </row>
+    <row r="240" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B240" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="C240" s="19"/>
+      <c r="D240" s="19"/>
+      <c r="E240" s="19"/>
+      <c r="F240" s="19"/>
+      <c r="G240" s="19"/>
+      <c r="H240" s="19"/>
+      <c r="I240" s="19"/>
+      <c r="J240" s="5"/>
+    </row>
+    <row r="241" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B241" s="4"/>
+      <c r="C241" s="19"/>
+      <c r="D241" s="19"/>
+      <c r="E241" s="19"/>
+      <c r="F241" s="19"/>
+      <c r="G241" s="19"/>
+      <c r="H241" s="19"/>
+      <c r="I241" s="19"/>
+      <c r="J241" s="5"/>
+    </row>
+    <row r="242" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B242" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="C242" s="19"/>
+      <c r="D242" s="19"/>
+      <c r="E242" s="19"/>
+      <c r="F242" s="19"/>
+      <c r="G242" s="19"/>
+      <c r="H242" s="19"/>
+      <c r="I242" s="19"/>
+      <c r="J242" s="5"/>
+    </row>
+    <row r="243" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B243" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="C243" s="19"/>
+      <c r="D243" s="19"/>
+      <c r="E243" s="19"/>
+      <c r="F243" s="19"/>
+      <c r="G243" s="19"/>
+      <c r="H243" s="19"/>
+      <c r="I243" s="19"/>
+      <c r="J243" s="5"/>
+    </row>
+    <row r="244" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B244" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="C244" s="19"/>
+      <c r="D244" s="19"/>
+      <c r="E244" s="19"/>
+      <c r="F244" s="19"/>
+      <c r="G244" s="19"/>
+      <c r="H244" s="19"/>
+      <c r="I244" s="19"/>
+      <c r="J244" s="5"/>
+    </row>
+    <row r="245" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B245" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="C245" s="19"/>
+      <c r="D245" s="19"/>
+      <c r="E245" s="19"/>
+      <c r="F245" s="19"/>
+      <c r="G245" s="19"/>
+      <c r="H245" s="19"/>
+      <c r="I245" s="19"/>
+      <c r="J245" s="5"/>
+    </row>
+    <row r="246" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B246" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="C246" s="19"/>
+      <c r="D246" s="19"/>
+      <c r="E246" s="19"/>
+      <c r="F246" s="19"/>
+      <c r="G246" s="19"/>
+      <c r="H246" s="19"/>
+      <c r="I246" s="19"/>
+      <c r="J246" s="5"/>
+    </row>
+    <row r="247" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B247" s="4"/>
+      <c r="C247" s="19"/>
+      <c r="D247" s="19"/>
+      <c r="E247" s="19"/>
+      <c r="F247" s="19"/>
+      <c r="G247" s="19"/>
+      <c r="H247" s="19"/>
+      <c r="I247" s="19"/>
+      <c r="J247" s="5"/>
+    </row>
+    <row r="248" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B248" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="C248" s="19"/>
+      <c r="D248" s="19"/>
+      <c r="E248" s="19"/>
+      <c r="F248" s="19"/>
+      <c r="G248" s="19"/>
+      <c r="H248" s="19"/>
+      <c r="I248" s="19"/>
+      <c r="J248" s="5"/>
+    </row>
+    <row r="249" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B249" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="C249" s="19"/>
+      <c r="D249" s="19"/>
+      <c r="E249" s="19"/>
+      <c r="F249" s="19"/>
+      <c r="G249" s="19"/>
+      <c r="H249" s="19"/>
+      <c r="I249" s="19"/>
+      <c r="J249" s="5"/>
+    </row>
+    <row r="250" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B250" s="4"/>
+      <c r="C250" s="19"/>
+      <c r="D250" s="19"/>
+      <c r="E250" s="19"/>
+      <c r="F250" s="19"/>
+      <c r="G250" s="19"/>
+      <c r="H250" s="19"/>
+      <c r="I250" s="19"/>
+      <c r="J250" s="5"/>
+    </row>
+    <row r="251" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B251" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="C251" s="19"/>
+      <c r="D251" s="19"/>
+      <c r="E251" s="19"/>
+      <c r="F251" s="19"/>
+      <c r="G251" s="19"/>
+      <c r="H251" s="19"/>
+      <c r="I251" s="19"/>
+      <c r="J251" s="5"/>
+    </row>
+    <row r="252" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B252" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="C252" s="19"/>
+      <c r="D252" s="19"/>
+      <c r="E252" s="19"/>
+      <c r="F252" s="19"/>
+      <c r="G252" s="19"/>
+      <c r="H252" s="19"/>
+      <c r="I252" s="19"/>
+      <c r="J252" s="5"/>
+    </row>
+    <row r="253" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B253" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="C253" s="19"/>
+      <c r="D253" s="19"/>
+      <c r="E253" s="19"/>
+      <c r="F253" s="19"/>
+      <c r="G253" s="19"/>
+      <c r="H253" s="19"/>
+      <c r="I253" s="19"/>
+      <c r="J253" s="5"/>
+    </row>
+    <row r="254" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B254" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="C254" s="19"/>
+      <c r="D254" s="19"/>
+      <c r="E254" s="19"/>
+      <c r="F254" s="19"/>
+      <c r="G254" s="19"/>
+      <c r="H254" s="19"/>
+      <c r="I254" s="19"/>
+      <c r="J254" s="5"/>
+    </row>
+    <row r="255" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B255" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="C255" s="19"/>
+      <c r="D255" s="19"/>
+      <c r="E255" s="19"/>
+      <c r="F255" s="19"/>
+      <c r="G255" s="19"/>
+      <c r="H255" s="19"/>
+      <c r="I255" s="19"/>
+      <c r="J255" s="5"/>
+    </row>
+    <row r="256" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B256" s="4" t="s">
+        <v>365</v>
+      </c>
+      <c r="C256" s="19"/>
+      <c r="D256" s="19"/>
+      <c r="E256" s="19"/>
+      <c r="F256" s="19"/>
+      <c r="G256" s="19"/>
+      <c r="H256" s="19"/>
+      <c r="I256" s="19"/>
+      <c r="J256" s="5"/>
+    </row>
+    <row r="257" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B257" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="C257" s="19"/>
+      <c r="D257" s="19"/>
+      <c r="E257" s="19"/>
+      <c r="F257" s="19"/>
+      <c r="G257" s="19"/>
+      <c r="H257" s="19"/>
+      <c r="I257" s="19"/>
+      <c r="J257" s="5"/>
+    </row>
+    <row r="258" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B258" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="C258" s="19"/>
+      <c r="D258" s="19"/>
+      <c r="E258" s="19"/>
+      <c r="F258" s="19"/>
+      <c r="G258" s="19"/>
+      <c r="H258" s="19"/>
+      <c r="I258" s="19"/>
+      <c r="J258" s="5"/>
+    </row>
+    <row r="259" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B259" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="C259" s="19"/>
+      <c r="D259" s="19"/>
+      <c r="E259" s="19"/>
+      <c r="F259" s="19"/>
+      <c r="G259" s="19"/>
+      <c r="H259" s="19"/>
+      <c r="I259" s="19"/>
+      <c r="J259" s="5"/>
+    </row>
+    <row r="260" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B260" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="C260" s="19"/>
+      <c r="D260" s="19"/>
+      <c r="E260" s="19"/>
+      <c r="F260" s="19"/>
+      <c r="G260" s="19"/>
+      <c r="H260" s="19"/>
+      <c r="I260" s="19"/>
+      <c r="J260" s="5"/>
+    </row>
+    <row r="261" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B261" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="C261" s="19"/>
+      <c r="D261" s="19"/>
+      <c r="E261" s="19"/>
+      <c r="F261" s="19"/>
+      <c r="G261" s="19"/>
+      <c r="H261" s="19"/>
+      <c r="I261" s="19"/>
+      <c r="J261" s="5"/>
+    </row>
+    <row r="262" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B262" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="C262" s="19"/>
+      <c r="D262" s="19"/>
+      <c r="E262" s="19"/>
+      <c r="F262" s="19"/>
+      <c r="G262" s="19"/>
+      <c r="H262" s="19"/>
+      <c r="I262" s="19"/>
+      <c r="J262" s="5"/>
+    </row>
+    <row r="263" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B263" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="C263" s="19"/>
+      <c r="D263" s="19"/>
+      <c r="E263" s="19"/>
+      <c r="F263" s="19"/>
+      <c r="G263" s="19"/>
+      <c r="H263" s="19"/>
+      <c r="I263" s="19"/>
+      <c r="J263" s="5"/>
+    </row>
+    <row r="264" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B264" s="4"/>
+      <c r="C264" s="19"/>
+      <c r="D264" s="19"/>
+      <c r="E264" s="19"/>
+      <c r="F264" s="19"/>
+      <c r="G264" s="19"/>
+      <c r="H264" s="19"/>
+      <c r="I264" s="19"/>
+      <c r="J264" s="5"/>
+    </row>
+    <row r="265" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B265" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="C265" s="19"/>
+      <c r="D265" s="19"/>
+      <c r="E265" s="19"/>
+      <c r="F265" s="19"/>
+      <c r="G265" s="19"/>
+      <c r="H265" s="19"/>
+      <c r="I265" s="19"/>
+      <c r="J265" s="5"/>
+    </row>
+    <row r="266" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B266" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="C266" s="19"/>
+      <c r="D266" s="19"/>
+      <c r="E266" s="19"/>
+      <c r="F266" s="19"/>
+      <c r="G266" s="19"/>
+      <c r="H266" s="19"/>
+      <c r="I266" s="19"/>
+      <c r="J266" s="5"/>
+    </row>
+    <row r="267" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B267" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="C267" s="19"/>
+      <c r="D267" s="19"/>
+      <c r="E267" s="19"/>
+      <c r="F267" s="19"/>
+      <c r="G267" s="19"/>
+      <c r="H267" s="19"/>
+      <c r="I267" s="19"/>
+      <c r="J267" s="5"/>
+    </row>
+    <row r="268" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B268" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="C268" s="19"/>
+      <c r="D268" s="19"/>
+      <c r="E268" s="19"/>
+      <c r="F268" s="19"/>
+      <c r="G268" s="19"/>
+      <c r="H268" s="19"/>
+      <c r="I268" s="19"/>
+      <c r="J268" s="5"/>
+    </row>
+    <row r="269" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B269" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="C269" s="19"/>
+      <c r="D269" s="19"/>
+      <c r="E269" s="19"/>
+      <c r="F269" s="19"/>
+      <c r="G269" s="19"/>
+      <c r="H269" s="19"/>
+      <c r="I269" s="19"/>
+      <c r="J269" s="5"/>
+    </row>
+    <row r="270" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B270" s="4"/>
+      <c r="C270" s="19"/>
+      <c r="D270" s="19"/>
+      <c r="E270" s="19"/>
+      <c r="F270" s="19"/>
+      <c r="G270" s="19"/>
+      <c r="H270" s="19"/>
+      <c r="I270" s="19"/>
+      <c r="J270" s="5"/>
+    </row>
+    <row r="271" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B271" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="C271" s="19"/>
+      <c r="D271" s="19"/>
+      <c r="E271" s="19"/>
+      <c r="F271" s="19"/>
+      <c r="G271" s="19"/>
+      <c r="H271" s="19"/>
+      <c r="I271" s="19"/>
+      <c r="J271" s="5"/>
+    </row>
+    <row r="272" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B272" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="C272" s="19"/>
+      <c r="D272" s="19"/>
+      <c r="E272" s="19"/>
+      <c r="F272" s="19"/>
+      <c r="G272" s="19"/>
+      <c r="H272" s="19"/>
+      <c r="I272" s="19"/>
+      <c r="J272" s="5"/>
+    </row>
+    <row r="273" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B273" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="C273" s="19"/>
+      <c r="D273" s="19"/>
+      <c r="E273" s="19"/>
+      <c r="F273" s="19"/>
+      <c r="G273" s="19"/>
+      <c r="H273" s="19"/>
+      <c r="I273" s="19"/>
+      <c r="J273" s="5"/>
+    </row>
+    <row r="274" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B274" s="4" t="s">
+        <v>373</v>
+      </c>
+      <c r="C274" s="19"/>
+      <c r="D274" s="19"/>
+      <c r="E274" s="19"/>
+      <c r="F274" s="19"/>
+      <c r="G274" s="19"/>
+      <c r="H274" s="19"/>
+      <c r="I274" s="19"/>
+      <c r="J274" s="5"/>
+    </row>
+    <row r="275" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B275" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="C275" s="19"/>
+      <c r="D275" s="19"/>
+      <c r="E275" s="19"/>
+      <c r="F275" s="19"/>
+      <c r="G275" s="19"/>
+      <c r="H275" s="19"/>
+      <c r="I275" s="19"/>
+      <c r="J275" s="5"/>
+    </row>
+    <row r="276" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B276" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="C276" s="19"/>
+      <c r="D276" s="19"/>
+      <c r="E276" s="19"/>
+      <c r="F276" s="19"/>
+      <c r="G276" s="19"/>
+      <c r="H276" s="19"/>
+      <c r="I276" s="19"/>
+      <c r="J276" s="5"/>
+    </row>
+    <row r="277" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B277" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="C277" s="19"/>
+      <c r="D277" s="19"/>
+      <c r="E277" s="19"/>
+      <c r="F277" s="19"/>
+      <c r="G277" s="19"/>
+      <c r="H277" s="19"/>
+      <c r="I277" s="19"/>
+      <c r="J277" s="5"/>
+    </row>
+    <row r="278" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B278" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="C278" s="19"/>
+      <c r="D278" s="19"/>
+      <c r="E278" s="19"/>
+      <c r="F278" s="19"/>
+      <c r="G278" s="19"/>
+      <c r="H278" s="19"/>
+      <c r="I278" s="19"/>
+      <c r="J278" s="5"/>
+    </row>
+    <row r="279" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B279" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="C279" s="19"/>
+      <c r="D279" s="19"/>
+      <c r="E279" s="19"/>
+      <c r="F279" s="19"/>
+      <c r="G279" s="19"/>
+      <c r="H279" s="19"/>
+      <c r="I279" s="19"/>
+      <c r="J279" s="5"/>
+    </row>
+    <row r="280" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B280" s="4"/>
+      <c r="C280" s="19"/>
+      <c r="D280" s="19"/>
+      <c r="E280" s="19"/>
+      <c r="F280" s="19"/>
+      <c r="G280" s="19"/>
+      <c r="H280" s="19"/>
+      <c r="I280" s="19"/>
+      <c r="J280" s="5"/>
+    </row>
+    <row r="281" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B281" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="C281" s="19"/>
+      <c r="D281" s="19"/>
+      <c r="E281" s="19"/>
+      <c r="F281" s="19"/>
+      <c r="G281" s="19"/>
+      <c r="H281" s="19"/>
+      <c r="I281" s="19"/>
+      <c r="J281" s="5"/>
+    </row>
+    <row r="282" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B282" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="C282" s="19"/>
+      <c r="D282" s="19"/>
+      <c r="E282" s="19"/>
+      <c r="F282" s="19"/>
+      <c r="G282" s="19"/>
+      <c r="H282" s="19"/>
+      <c r="I282" s="19"/>
+      <c r="J282" s="5"/>
+    </row>
+    <row r="283" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B283" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="C283" s="19"/>
+      <c r="D283" s="19"/>
+      <c r="E283" s="19"/>
+      <c r="F283" s="19"/>
+      <c r="G283" s="19"/>
+      <c r="H283" s="19"/>
+      <c r="I283" s="19"/>
+      <c r="J283" s="5"/>
+    </row>
+    <row r="284" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B284" s="4" t="s">
+        <v>378</v>
+      </c>
+      <c r="C284" s="19"/>
+      <c r="D284" s="19"/>
+      <c r="E284" s="19"/>
+      <c r="F284" s="19"/>
+      <c r="G284" s="19"/>
+      <c r="H284" s="19"/>
+      <c r="I284" s="19"/>
+      <c r="J284" s="5"/>
+    </row>
+    <row r="285" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B285" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="C285" s="19"/>
+      <c r="D285" s="19"/>
+      <c r="E285" s="19"/>
+      <c r="F285" s="19"/>
+      <c r="G285" s="19"/>
+      <c r="H285" s="19"/>
+      <c r="I285" s="19"/>
+      <c r="J285" s="5"/>
+    </row>
+    <row r="286" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B286" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="C286" s="19"/>
+      <c r="D286" s="19"/>
+      <c r="E286" s="19"/>
+      <c r="F286" s="19"/>
+      <c r="G286" s="19"/>
+      <c r="H286" s="19"/>
+      <c r="I286" s="19"/>
+      <c r="J286" s="5"/>
+    </row>
+    <row r="287" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B287" s="4"/>
+      <c r="C287" s="19"/>
+      <c r="D287" s="19"/>
+      <c r="E287" s="19"/>
+      <c r="F287" s="19"/>
+      <c r="G287" s="19"/>
+      <c r="H287" s="19"/>
+      <c r="I287" s="19"/>
+      <c r="J287" s="5"/>
+    </row>
+    <row r="288" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B288" s="21" t="s">
+        <v>423</v>
+      </c>
+      <c r="C288" s="2"/>
+      <c r="D288" s="2"/>
+      <c r="E288" s="2"/>
+      <c r="F288" s="2"/>
+      <c r="G288" s="2"/>
+      <c r="H288" s="2"/>
+      <c r="I288" s="2"/>
+      <c r="J288" s="3"/>
+    </row>
+    <row r="289" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B289" s="20" t="s">
+        <v>424</v>
+      </c>
+      <c r="C289" s="19"/>
+      <c r="D289" s="19"/>
+      <c r="E289" s="19"/>
+      <c r="F289" s="19"/>
+      <c r="G289" s="19"/>
+      <c r="H289" s="19"/>
+      <c r="I289" s="19"/>
+      <c r="J289" s="5"/>
+    </row>
+    <row r="290" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B290" s="20" t="s">
+        <v>425</v>
+      </c>
+      <c r="C290" s="19"/>
+      <c r="D290" s="19"/>
+      <c r="E290" s="19"/>
+      <c r="F290" s="19"/>
+      <c r="G290" s="19"/>
+      <c r="H290" s="19"/>
+      <c r="I290" s="19"/>
+      <c r="J290" s="5"/>
+    </row>
+    <row r="291" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B291" s="20" t="s">
+        <v>323</v>
+      </c>
+      <c r="C291" s="19"/>
+      <c r="D291" s="19"/>
+      <c r="E291" s="19"/>
+      <c r="F291" s="19"/>
+      <c r="G291" s="19"/>
+      <c r="H291" s="19"/>
+      <c r="I291" s="19"/>
+      <c r="J291" s="5"/>
+    </row>
+    <row r="292" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B292" s="20" t="s">
+        <v>426</v>
+      </c>
+      <c r="C292" s="19"/>
+      <c r="D292" s="19"/>
+      <c r="E292" s="19"/>
+      <c r="F292" s="19"/>
+      <c r="G292" s="19"/>
+      <c r="H292" s="19"/>
+      <c r="I292" s="19"/>
+      <c r="J292" s="5"/>
+    </row>
+    <row r="293" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B293" s="20" t="s">
+        <v>325</v>
+      </c>
+      <c r="C293" s="19"/>
+      <c r="D293" s="19"/>
+      <c r="E293" s="19"/>
+      <c r="F293" s="19"/>
+      <c r="G293" s="19"/>
+      <c r="H293" s="19"/>
+      <c r="I293" s="19"/>
+      <c r="J293" s="5"/>
+    </row>
+    <row r="294" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B294" s="20" t="s">
+        <v>194</v>
+      </c>
+      <c r="C294" s="19"/>
+      <c r="D294" s="19"/>
+      <c r="E294" s="19"/>
+      <c r="F294" s="19"/>
+      <c r="G294" s="19"/>
+      <c r="H294" s="19"/>
+      <c r="I294" s="19"/>
+      <c r="J294" s="5"/>
+    </row>
+    <row r="295" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B295" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="C295" s="19"/>
+      <c r="D295" s="19"/>
+      <c r="E295" s="19"/>
+      <c r="F295" s="19"/>
+      <c r="G295" s="19"/>
+      <c r="H295" s="19"/>
+      <c r="I295" s="19"/>
+      <c r="J295" s="5"/>
+    </row>
+    <row r="296" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B296" s="26" t="s">
+        <v>208</v>
+      </c>
+      <c r="C296" s="8"/>
+      <c r="D296" s="8"/>
+      <c r="E296" s="8"/>
+      <c r="F296" s="8"/>
+      <c r="G296" s="8"/>
+      <c r="H296" s="8"/>
+      <c r="I296" s="8"/>
+      <c r="J296" s="9"/>
+    </row>
+    <row r="299" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A299" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="300" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B300" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="C300" s="2"/>
+      <c r="D300" s="2"/>
+      <c r="E300" s="2"/>
+      <c r="F300" s="3"/>
+    </row>
+    <row r="301" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B301" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="C301" s="19"/>
+      <c r="D301" s="19"/>
+      <c r="E301" s="19"/>
+      <c r="F301" s="5"/>
+    </row>
+    <row r="302" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B302" s="4"/>
+      <c r="C302" s="19"/>
+      <c r="D302" s="19"/>
+      <c r="E302" s="19"/>
+      <c r="F302" s="5"/>
+    </row>
+    <row r="303" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B303" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="C303" s="19"/>
+      <c r="D303" s="19"/>
+      <c r="E303" s="19"/>
+      <c r="F303" s="5"/>
+    </row>
+    <row r="304" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B304" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="C304" s="19"/>
+      <c r="D304" s="19"/>
+      <c r="E304" s="19"/>
+      <c r="F304" s="5"/>
+    </row>
+    <row r="305" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B305" s="4" t="s">
+        <v>384</v>
+      </c>
+      <c r="C305" s="19"/>
+      <c r="D305" s="19"/>
+      <c r="E305" s="19"/>
+      <c r="F305" s="5"/>
+    </row>
+    <row r="306" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B306" s="4" t="s">
+        <v>385</v>
+      </c>
+      <c r="C306" s="19"/>
+      <c r="D306" s="19"/>
+      <c r="E306" s="19"/>
+      <c r="F306" s="5"/>
+    </row>
+    <row r="307" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B307" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="C307" s="19"/>
+      <c r="D307" s="19"/>
+      <c r="E307" s="19"/>
+      <c r="F307" s="5"/>
+    </row>
+    <row r="308" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B308" s="20" t="s">
+        <v>427</v>
+      </c>
+      <c r="C308" s="19"/>
+      <c r="D308" s="19"/>
+      <c r="E308" s="19"/>
+      <c r="F308" s="5"/>
+    </row>
+    <row r="309" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B309" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="C309" s="8"/>
+      <c r="D309" s="8"/>
+      <c r="E309" s="8"/>
+      <c r="F309" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>